<commit_message>
Updated remote server experiment files
</commit_message>
<xml_diff>
--- a/Remote experiments/Time scaling experiment results.xlsx
+++ b/Remote experiments/Time scaling experiment results.xlsx
@@ -16,13 +16,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>1.62 s ± 6.54 ms per loop (mean ± std. dev. of 10 runs, 1 loop each)</t>
+    <t>1.62 s ± 5.83 ms per loop (mean ± std. dev. of 10 runs, 1 loop each)</t>
   </si>
   <si>
-    <t>8.88 s ± 44 ms per loop (mean ± std. dev. of 10 runs, 1 loop each)</t>
+    <t>8.92 s ± 60.8 ms per loop (mean ± std. dev. of 10 runs, 1 loop each)</t>
   </si>
   <si>
-    <t>1.89 s ± 11.4 ms per loop (mean ± std. dev. of 10 runs, 1 loop each)</t>
+    <t>1.9 s ± 12.1 ms per loop (mean ± std. dev. of 10 runs, 1 loop each)</t>
   </si>
 </sst>
 </file>

</xml_diff>